<commit_message>
Uniquified directory structure and new top-level README
</commit_message>
<xml_diff>
--- a/S6_ASSIGNMENT/Normalizations.xlsx
+++ b/S6_ASSIGNMENT/Normalizations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75df4e63fbd4d7c9/EVA6/S6_ASSIGNMENT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{44184509-2164-49B6-B435-299F0B635CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{066AFA6A-AAAD-4D1D-AA49-A0B36CB80B00}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{44184509-2164-49B6-B435-299F0B635CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FD58617-AC99-4854-B6D3-94751E69C4DE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4BC243D-02FB-45C5-9A4D-F620BC3AB2C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4BC243D-02FB-45C5-9A4D-F620BC3AB2C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Layer N</t>
   </si>
@@ -73,6 +73,36 @@
   </si>
   <si>
     <t>μ_i_g</t>
+  </si>
+  <si>
+    <t>IMG1</t>
+  </si>
+  <si>
+    <t>LAYER</t>
+  </si>
+  <si>
+    <t>IMG2</t>
+  </si>
+  <si>
+    <t>Batch Norm</t>
+  </si>
+  <si>
+    <t>CHANNEL1</t>
+  </si>
+  <si>
+    <t>CHANNEL2</t>
+  </si>
+  <si>
+    <t>CHANNEL3</t>
+  </si>
+  <si>
+    <t>LayerNorm</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>GroupNorm</t>
   </si>
 </sst>
 </file>
@@ -161,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -249,92 +279,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -354,11 +368,104 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -386,13 +493,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -450,13 +557,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -514,13 +621,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -578,13 +685,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -642,13 +749,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -711,13 +818,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -780,13 +887,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -849,13 +956,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -918,13 +1025,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -988,13 +1095,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -1058,13 +1165,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -1128,13 +1235,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -1198,13 +1305,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -1262,13 +1369,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1326,13 +1433,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1390,13 +1497,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1454,13 +1561,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1518,13 +1625,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1582,13 +1689,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1646,13 +1753,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1710,13 +1817,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1779,13 +1886,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1848,13 +1955,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1917,13 +2024,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1986,13 +2093,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2055,13 +2162,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2124,13 +2231,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2193,13 +2300,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2262,13 +2369,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2332,13 +2439,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2402,13 +2509,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2472,13 +2579,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2542,13 +2649,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2612,13 +2719,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2682,13 +2789,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2752,13 +2859,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2822,16 +2929,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>100965</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2846,8 +2953,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6143625" y="5648325"/>
-          <a:ext cx="1743075" cy="180975"/>
+          <a:off x="8848725" y="5695950"/>
+          <a:ext cx="1788795" cy="188595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2886,13 +2993,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>598170</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>211455</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -2950,13 +3057,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -3014,13 +3121,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -3078,13 +3185,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -3440,1812 +3547,1323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C7F0F4-C027-424B-B3B0-C0F7367A4E4F}">
-  <dimension ref="E2:AJ37"/>
+  <dimension ref="A4:AL36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="9" width="9.109375" style="2"/>
-    <col min="10" max="10" width="9.109375" style="2" customWidth="1"/>
-    <col min="11" max="12" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="2" customWidth="1"/>
-    <col min="14" max="15" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="2"/>
-    <col min="17" max="18" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" style="2"/>
-    <col min="20" max="20" width="4" style="2" customWidth="1"/>
-    <col min="21" max="21" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.109375" style="2"/>
-    <col min="23" max="23" width="9.109375" style="2" customWidth="1"/>
-    <col min="24" max="24" width="3.6640625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.109375" style="2" customWidth="1"/>
-    <col min="27" max="28" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.109375" style="2" customWidth="1"/>
-    <col min="30" max="30" width="4.109375" style="2" customWidth="1"/>
-    <col min="31" max="31" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.109375" style="2" customWidth="1"/>
-    <col min="33" max="34" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="13" width="9.109375" style="9"/>
+    <col min="14" max="14" width="9.109375" style="9" customWidth="1"/>
+    <col min="15" max="16" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="9" customWidth="1"/>
+    <col min="18" max="19" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" style="9"/>
+    <col min="21" max="22" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" style="9"/>
+    <col min="24" max="24" width="4" style="9" customWidth="1"/>
+    <col min="25" max="25" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" style="9"/>
+    <col min="27" max="27" width="9.109375" style="9" customWidth="1"/>
+    <col min="28" max="28" width="3.6640625" style="9" customWidth="1"/>
+    <col min="29" max="29" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.109375" style="9" customWidth="1"/>
+    <col min="31" max="32" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.109375" style="9" customWidth="1"/>
+    <col min="34" max="34" width="4.109375" style="9" customWidth="1"/>
+    <col min="35" max="35" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.109375" style="9" customWidth="1"/>
+    <col min="37" max="38" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:36">
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
+    <row r="4" spans="1:38">
+      <c r="O4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="AB4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
     </row>
-    <row r="3" spans="5:36">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
+    <row r="5" spans="1:38">
+      <c r="C5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
-    <row r="4" spans="5:36">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="17" t="s">
+    <row r="6" spans="1:38" ht="16.2" thickBot="1">
+      <c r="C6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:38" ht="16.2" thickBot="1">
+      <c r="B7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="11">
+        <v>4</v>
+      </c>
+      <c r="D7" s="12">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11">
+        <v>-2</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="17"/>
+      <c r="M7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="18">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="17" t="s">
+      <c r="P7" s="19">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>4</v>
+      </c>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>-2</v>
+      </c>
+      <c r="S7" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>3</v>
+      </c>
+      <c r="T7" s="20"/>
+      <c r="U7" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
         <v>1</v>
       </c>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
+      <c r="V7" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="20"/>
+      <c r="X7" s="23">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="Y7" s="24">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AB7" s="18">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-1</v>
+      </c>
+      <c r="AC7" s="19">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="21">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AF7" s="21">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="22">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-1</v>
+      </c>
+      <c r="AI7" s="22">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="23">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AL7" s="24">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="5:36">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-    </row>
-    <row r="6" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-    </row>
-    <row r="7" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E7" s="1"/>
-      <c r="F7" s="35" t="s">
+    <row r="8" spans="1:38" ht="16.2" thickBot="1">
+      <c r="B8" s="10"/>
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
+      <c r="D8" s="14">
         <v>5</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="23" t="s">
+      <c r="E8" s="13">
+        <v>4</v>
+      </c>
+      <c r="F8" s="14">
+        <v>6</v>
+      </c>
+      <c r="G8" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="14">
         <v>2</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="3">
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="M8" s="10"/>
+      <c r="O8" s="18">
         <f ca="1">RANDBETWEEN(-4, 4)</f>
         <v>2</v>
       </c>
-      <c r="L7" s="4">
+      <c r="P8" s="19">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>-1</v>
+      </c>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>1</v>
+      </c>
+      <c r="S8" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>-3</v>
+      </c>
+      <c r="T8" s="25"/>
+      <c r="U8" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>-4</v>
+      </c>
+      <c r="V8" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="W8" s="25"/>
+      <c r="X8" s="26">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="Y8" s="27">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AB8" s="28">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="AC8" s="29">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="30">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AF8" s="30">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="31">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AI8" s="31">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AJ8" s="25"/>
+      <c r="AK8" s="26">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="AL8" s="27">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="16.2" thickBot="1">
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:38" ht="16.2" thickBot="1">
+      <c r="B10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12">
+        <v>4</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="M10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="18">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>3</v>
+      </c>
+      <c r="P10" s="19">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>-4</v>
+      </c>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>-2</v>
+      </c>
+      <c r="S10" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="20"/>
+      <c r="U10" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>-3</v>
+      </c>
+      <c r="V10" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="W10" s="20"/>
+      <c r="X10" s="23">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="Y10" s="24">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AB10" s="18">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AC10" s="19">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="21">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="AF10" s="21">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="22">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AI10" s="22">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="23">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="AL10" s="24">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="16.2" thickBot="1">
+      <c r="B11" s="10"/>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>3</v>
+      </c>
+      <c r="E11" s="13">
+        <v>4</v>
+      </c>
+      <c r="F11" s="14">
+        <v>5</v>
+      </c>
+      <c r="G11" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="M11" s="10"/>
+      <c r="O11" s="18">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>3</v>
+      </c>
+      <c r="P11" s="19">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>-4</v>
+      </c>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>-2</v>
+      </c>
+      <c r="S11" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="25"/>
+      <c r="U11" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>-3</v>
+      </c>
+      <c r="V11" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>-3</v>
+      </c>
+      <c r="W11" s="25"/>
+      <c r="X11" s="26">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-1</v>
+      </c>
+      <c r="Y11" s="27">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AB11" s="28">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="AC11" s="29">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AD11" s="25"/>
+      <c r="AE11" s="30">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="AF11" s="30">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="25"/>
+      <c r="AH11" s="31">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AI11" s="31">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AJ11" s="25"/>
+      <c r="AK11" s="26">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-1</v>
+      </c>
+      <c r="AL11" s="27">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="16.2" thickBot="1">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="32">
+        <f>AVERAGE(C7:D11)</f>
+        <v>3.25</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32">
+        <f>AVERAGE(E7:F11)</f>
+        <v>2.625</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32">
+        <f>AVERAGE(G7:H11)</f>
+        <v>0.375</v>
+      </c>
+      <c r="H12" s="32"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:38" ht="16.2" thickBot="1">
+      <c r="A13" s="1"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="M13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" s="18">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="19">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>4</v>
+      </c>
+      <c r="S13" s="21">
         <f ca="1">RANDBETWEEN(-4, 4)</f>
         <v>2</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="6">
+      <c r="T13" s="20"/>
+      <c r="U13" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>-3</v>
+      </c>
+      <c r="V13" s="22">
+        <f ca="1">RANDBETWEEN(-4, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="W13" s="20"/>
+      <c r="X13" s="23">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="24">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AB13" s="18">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="19">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="21">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AF13" s="21">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="22">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AI13" s="22">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-1</v>
+      </c>
+      <c r="AJ13" s="20"/>
+      <c r="AK13" s="23">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AL13" s="24">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="16.2" thickBot="1">
+      <c r="A14" s="1"/>
+      <c r="C14" s="10">
+        <f>_xlfn.VAR.P(C7:D11)</f>
+        <v>1.4375</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10">
+        <f>_xlfn.VAR.P(E7:F11)</f>
+        <v>5.984375</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10">
+        <f>_xlfn.VAR.P(G7:H11)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="M14" s="10"/>
+      <c r="O14" s="18">
         <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>2</v>
-      </c>
-      <c r="O7" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="19">
         <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>3</v>
-      </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>-4</v>
-      </c>
-      <c r="R7" s="7">
+        <v>-3</v>
+      </c>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>4</v>
+      </c>
+      <c r="S14" s="21">
+        <f ca="1">RANDBETWEEN(-4, 4)</f>
+        <v>1</v>
+      </c>
+      <c r="T14" s="25"/>
+      <c r="U14" s="22">
         <f ca="1">RANDBETWEEN(-4, 2)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="5"/>
-      <c r="T7" s="8">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="U7" s="9">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="3">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="4">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="6">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="AB7" s="6">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="7">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="AE7" s="7">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>2</v>
-      </c>
-      <c r="AF7" s="5"/>
-      <c r="AG7" s="8">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="9">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-    </row>
-    <row r="8" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E8" s="1"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-3</v>
-      </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>4</v>
-      </c>
-      <c r="O8" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-3</v>
-      </c>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>0</v>
-      </c>
-      <c r="R8" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>-3</v>
-      </c>
-      <c r="S8" s="12"/>
-      <c r="T8" s="15">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="U8" s="16">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>2</v>
-      </c>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="10">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="11">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>2</v>
-      </c>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="13">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-1</v>
-      </c>
-      <c r="AB8" s="13">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-1</v>
-      </c>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="14">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="AE8" s="14">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-1</v>
-      </c>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="15">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AH8" s="16">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-    </row>
-    <row r="9" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E9" s="1"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-    </row>
-    <row r="10" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E10" s="1"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="3">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>3</v>
-      </c>
-      <c r="L10" s="4">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-3</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>3</v>
-      </c>
-      <c r="O10" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>2</v>
-      </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>-4</v>
-      </c>
-      <c r="R10" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>-1</v>
-      </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="8">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="U10" s="9">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="3">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="Y10" s="4">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="6">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>2</v>
-      </c>
-      <c r="AB10" s="6">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="7">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="AE10" s="7">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="8">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-1</v>
-      </c>
-      <c r="AH10" s="9">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-    </row>
-    <row r="11" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E11" s="1"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="3">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>3</v>
-      </c>
-      <c r="L11" s="4">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-1</v>
-      </c>
-      <c r="M11" s="12"/>
-      <c r="N11" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>2</v>
-      </c>
-      <c r="O11" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>3</v>
-      </c>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>0</v>
-      </c>
-      <c r="S11" s="12"/>
-      <c r="T11" s="15">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>2</v>
-      </c>
-      <c r="U11" s="16">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="10">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="Y11" s="11">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="13">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>2</v>
-      </c>
-      <c r="AB11" s="13">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-1</v>
-      </c>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="14">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="AE11" s="14">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AF11" s="12"/>
-      <c r="AG11" s="15">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="AH11" s="16">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-    </row>
-    <row r="12" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E12" s="1"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-    </row>
-    <row r="13" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E13" s="1"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="3">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-3</v>
-      </c>
-      <c r="L13" s="4">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-1</v>
-      </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>3</v>
-      </c>
-      <c r="O13" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-3</v>
-      </c>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="7">
+      <c r="V14" s="22">
         <f ca="1">RANDBETWEEN(-4, 2)</f>
         <v>-2</v>
       </c>
-      <c r="R13" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
+      <c r="W14" s="25"/>
+      <c r="X14" s="26">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
         <v>-1</v>
       </c>
-      <c r="S13" s="5"/>
-      <c r="T13" s="8">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
+      <c r="Y14" s="27">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AB14" s="28">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AC14" s="29">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AD14" s="25"/>
+      <c r="AE14" s="30">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AF14" s="30">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AG14" s="25"/>
+      <c r="AH14" s="31">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AI14" s="31">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="AJ14" s="25"/>
+      <c r="AK14" s="26">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-2</v>
+      </c>
+      <c r="AL14" s="27">
+        <f ca="1">RANDBETWEEN(-3, 3)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38">
+      <c r="A15" s="1"/>
+      <c r="B15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="17" spans="1:38">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="10">
+        <f>AVERAGE(C7:H8)</f>
+        <v>2.4166666666666665</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="F17" s="10">
+        <f>AVERAGE(C10:H11)</f>
+        <v>1.75</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="J17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="33">
+        <f ca="1">AVERAGE(O7:P8,O10:P11,O13:P14)</f>
         <v>0</v>
       </c>
-      <c r="U13" s="9">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
+      <c r="P17" s="33"/>
+      <c r="R17" s="34">
+        <f ca="1">AVERAGE(R7:S8,R10:S11,R13:S14)</f>
+        <v>0.5</v>
+      </c>
+      <c r="S17" s="34"/>
+      <c r="U17" s="35">
+        <f ca="1">AVERAGE(U7:V8,U10:V11,U13:V14)</f>
+        <v>-1.0833333333333333</v>
+      </c>
+      <c r="V17" s="35"/>
+      <c r="X17" s="36">
+        <f ca="1">AVERAGE(X7:Y8,X10:Y11,X13:Y14)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="Y17" s="36"/>
+      <c r="AB17" s="33">
+        <f ca="1">AVERAGE(AB7:AC8,AB10:AC11,AB13:AC14)</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="AC17" s="33"/>
+      <c r="AE17" s="34">
+        <f ca="1">AVERAGE(AE7:AF8,AE10:AF11,AE13:AF14)</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="AF17" s="34"/>
+      <c r="AH17" s="35">
+        <f ca="1">AVERAGE(AH7:AI8,AH10:AI11,AH13:AI14)</f>
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="AI17" s="35"/>
+      <c r="AK17" s="36">
+        <f ca="1">AVERAGE(AK7:AL8,AK10:AL11,AK13:AL14)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="AL17" s="36"/>
+    </row>
+    <row r="18" spans="1:38">
+      <c r="A18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="33"/>
+      <c r="AE18" s="34"/>
+      <c r="AF18" s="34"/>
+      <c r="AH18" s="35"/>
+      <c r="AI18" s="35"/>
+      <c r="AK18" s="36"/>
+      <c r="AL18" s="36"/>
+    </row>
+    <row r="19" spans="1:38">
+      <c r="A19" s="1"/>
+      <c r="B19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="10">
+        <f>_xlfn.VAR.P(C7:H8)</f>
+        <v>5.2430555555555554</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="F19" s="10">
+        <f>_xlfn.VAR.P(C10:H11)</f>
+        <v>3.1875</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:38">
+      <c r="A20" s="1"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" s="33">
+        <f ca="1">_xlfn.VAR.P(O7:P8,O10:P11,O13:P14)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="P20" s="33"/>
+      <c r="R20" s="34">
+        <f ca="1">_xlfn.VAR.P(R7:S8,R10:S11,R13:S14)</f>
+        <v>5.416666666666667</v>
+      </c>
+      <c r="S20" s="34"/>
+      <c r="U20" s="35">
+        <f ca="1">_xlfn.VAR.P(U7:V8,U10:V11,U13:V14)</f>
+        <v>4.0763888888888893</v>
+      </c>
+      <c r="V20" s="35"/>
+      <c r="X20" s="36">
+        <f ca="1">_xlfn.VAR.P(X7:Y8,X10:Y11,X13:Y14)</f>
+        <v>3.0763888888888888</v>
+      </c>
+      <c r="Y20" s="36"/>
+      <c r="AB20" s="33">
+        <f ca="1">_xlfn.VAR.P(AB7:AC8,AB10:AC11,AB13:AC14)</f>
+        <v>4.0763888888888893</v>
+      </c>
+      <c r="AC20" s="33"/>
+      <c r="AE20" s="34">
+        <f ca="1">_xlfn.VAR.P(AE7:AF8,AE10:AF11,AE13:AF14)</f>
+        <v>5.4097222222222223</v>
+      </c>
+      <c r="AF20" s="34"/>
+      <c r="AH20" s="35">
+        <f ca="1">_xlfn.VAR.P(AH7:AI8,AH10:AI11,AH13:AI14)</f>
+        <v>4.9097222222222223</v>
+      </c>
+      <c r="AI20" s="35"/>
+      <c r="AK20" s="36">
+        <f ca="1">_xlfn.VAR.P(AK7:AL8,AK10:AL11,AK13:AL14)</f>
+        <v>3.6388888888888888</v>
+      </c>
+      <c r="AL20" s="36"/>
+    </row>
+    <row r="21" spans="1:38">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36"/>
+      <c r="AB21" s="33"/>
+      <c r="AC21" s="33"/>
+      <c r="AE21" s="34"/>
+      <c r="AF21" s="34"/>
+      <c r="AH21" s="35"/>
+      <c r="AI21" s="35"/>
+      <c r="AK21" s="36"/>
+      <c r="AL21" s="36"/>
+    </row>
+    <row r="22" spans="1:38" ht="16.2" thickBot="1">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:38">
+      <c r="A23" s="1"/>
+      <c r="B23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O23" s="37">
+        <f ca="1">AVERAGE(O7:Y8)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="38"/>
+      <c r="R23" s="37">
+        <f ca="1">AVERAGE(O10:Y11)</f>
+        <v>-0.8125</v>
+      </c>
+      <c r="S23" s="38"/>
+      <c r="U23" s="37">
+        <f ca="1">AVERAGE(O13:Y14)</f>
+        <v>0.4375</v>
+      </c>
+      <c r="V23" s="38"/>
+      <c r="AB23" s="37">
+        <f ca="1">AVERAGE(AB7:AL8)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="AC23" s="38"/>
+      <c r="AE23" s="37">
+        <f ca="1">AVERAGE(AB10:AL11)</f>
+        <v>-0.3125</v>
+      </c>
+      <c r="AF23" s="38"/>
+      <c r="AH23" s="37">
+        <f ca="1">AVERAGE(AB13:AL14)</f>
+        <v>-0.5625</v>
+      </c>
+      <c r="AI23" s="38"/>
+    </row>
+    <row r="24" spans="1:38" ht="16.2" thickBot="1">
+      <c r="A24" s="1"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="5"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="40"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="40"/>
+      <c r="U24" s="39"/>
+      <c r="V24" s="40"/>
+      <c r="AB24" s="39"/>
+      <c r="AC24" s="40"/>
+      <c r="AE24" s="39"/>
+      <c r="AF24" s="40"/>
+      <c r="AH24" s="39"/>
+      <c r="AI24" s="40"/>
+    </row>
+    <row r="25" spans="1:38" ht="16.2" thickBot="1">
+      <c r="J25" s="4"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:38" ht="16.2" thickBot="1">
+      <c r="J26" s="6"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O26" s="37">
+        <f ca="1">_xlfn.VAR.P(O7:Y8)</f>
+        <v>5</v>
+      </c>
+      <c r="P26" s="38"/>
+      <c r="R26" s="37">
+        <f ca="1">_xlfn.VAR.P(O10:Y11)</f>
+        <v>5.52734375</v>
+      </c>
+      <c r="S26" s="38"/>
+      <c r="U26" s="37">
+        <f ca="1">_xlfn.VAR.P(O13:Y14)</f>
+        <v>4.12109375</v>
+      </c>
+      <c r="V26" s="38"/>
+      <c r="AB26" s="37">
+        <f ca="1">_xlfn.VAR.P(AB7:AL8)</f>
+        <v>4.37109375</v>
+      </c>
+      <c r="AC26" s="38"/>
+      <c r="AE26" s="37">
+        <f ca="1">_xlfn.VAR.P(AB10:AL11)</f>
+        <v>3.83984375</v>
+      </c>
+      <c r="AF26" s="38"/>
+      <c r="AH26" s="37">
+        <f ca="1">_xlfn.VAR.P(AB13:AL14)</f>
+        <v>4.74609375</v>
+      </c>
+      <c r="AI26" s="38"/>
+    </row>
+    <row r="27" spans="1:38" ht="16.2" thickBot="1">
+      <c r="O27" s="39"/>
+      <c r="P27" s="40"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="40"/>
+      <c r="U27" s="39"/>
+      <c r="V27" s="40"/>
+      <c r="AB27" s="39"/>
+      <c r="AC27" s="40"/>
+      <c r="AE27" s="39"/>
+      <c r="AF27" s="40"/>
+      <c r="AH27" s="39"/>
+      <c r="AI27" s="40"/>
+    </row>
+    <row r="30" spans="1:38">
+      <c r="J30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" s="10">
+        <f ca="1">AVERAGE(O7:S8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="U30" s="10">
+        <f ca="1">AVERAGE(U7:Y8)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="AB30" s="10">
+        <f ca="1">AVERAGE(AB7:AF8)</f>
+        <v>0.25</v>
+      </c>
+      <c r="AC30" s="10"/>
+      <c r="AD30" s="10"/>
+      <c r="AE30" s="10"/>
+      <c r="AF30" s="10"/>
+      <c r="AH30" s="10">
+        <f ca="1">AVERAGE(AH7:AL8)</f>
+        <v>0.875</v>
+      </c>
+      <c r="AI30" s="10"/>
+      <c r="AJ30" s="10"/>
+      <c r="AK30" s="10"/>
+      <c r="AL30" s="10"/>
+    </row>
+    <row r="31" spans="1:38">
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="M31" s="10"/>
+      <c r="O31" s="10">
+        <f ca="1">AVERAGE(O10:S11)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="U31" s="10">
+        <f ca="1">AVERAGE(U10:Y11)</f>
+        <v>-0.875</v>
+      </c>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="AB31" s="10">
+        <f ca="1">AVERAGE(AB10:AF11)</f>
+        <v>0.25</v>
+      </c>
+      <c r="AC31" s="10"/>
+      <c r="AD31" s="10"/>
+      <c r="AE31" s="10"/>
+      <c r="AF31" s="10"/>
+      <c r="AH31" s="10">
+        <f ca="1">AVERAGE(AH10:AL11)</f>
+        <v>-0.875</v>
+      </c>
+      <c r="AI31" s="10"/>
+      <c r="AJ31" s="10"/>
+      <c r="AK31" s="10"/>
+      <c r="AL31" s="10"/>
+    </row>
+    <row r="32" spans="1:38">
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="M32" s="10"/>
+      <c r="O32" s="10">
+        <f ca="1">AVERAGE(O13:S14)</f>
         <v>1</v>
       </c>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="3">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="Y13" s="4">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-1</v>
-      </c>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="6">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="AB13" s="6">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="7">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>1</v>
-      </c>
-      <c r="AE13" s="7">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AF13" s="5"/>
-      <c r="AG13" s="8">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="AH13" s="9">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="U32" s="10">
+        <f ca="1">AVERAGE(U13:Y14)</f>
+        <v>-0.125</v>
+      </c>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10"/>
+      <c r="AB32" s="10">
+        <f ca="1">AVERAGE(AB13:AF14)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="AC32" s="10"/>
+      <c r="AD32" s="10"/>
+      <c r="AE32" s="10"/>
+      <c r="AF32" s="10"/>
+      <c r="AH32" s="10">
+        <f ca="1">AVERAGE(AH13:AL14)</f>
+        <v>-0.375</v>
+      </c>
+      <c r="AI32" s="10"/>
+      <c r="AJ32" s="10"/>
+      <c r="AK32" s="10"/>
+      <c r="AL32" s="10"/>
     </row>
-    <row r="14" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E14" s="1"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="3">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>-1</v>
-      </c>
-      <c r="L14" s="4">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>2</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>4</v>
-      </c>
-      <c r="O14" s="6">
-        <f ca="1">RANDBETWEEN(-4, 4)</f>
-        <v>4</v>
-      </c>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>-3</v>
-      </c>
-      <c r="R14" s="7">
-        <f ca="1">RANDBETWEEN(-4, 2)</f>
-        <v>-3</v>
-      </c>
-      <c r="S14" s="12"/>
-      <c r="T14" s="15">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="U14" s="16">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-3</v>
-      </c>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="10">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="Y14" s="11">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="13">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="13">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>3</v>
-      </c>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="14">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AE14" s="14">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="15">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-2</v>
-      </c>
-      <c r="AH14" s="16">
-        <f ca="1">RANDBETWEEN(-3, 3)</f>
-        <v>-1</v>
-      </c>
-      <c r="AI14" s="1"/>
-      <c r="AJ14" s="1"/>
-    </row>
-    <row r="15" spans="5:36">
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
-      <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
-      <c r="AJ15" s="1"/>
-    </row>
-    <row r="16" spans="5:36">
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="1"/>
-      <c r="AI16" s="1"/>
-      <c r="AJ16" s="1"/>
-    </row>
-    <row r="17" spans="5:36">
-      <c r="E17" s="1"/>
-      <c r="F17" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="19">
-        <f ca="1">AVERAGE(K7:L8,K10:L11,K13:L14)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="20">
-        <f ca="1">AVERAGE(N7:O8,N10:O11,N13:O14)</f>
-        <v>2</v>
-      </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="21">
-        <f ca="1">AVERAGE(Q7:R8,Q10:R11,Q13:R14)</f>
-        <v>-1.75</v>
-      </c>
-      <c r="R17" s="21"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="18">
-        <f ca="1">AVERAGE(T7:U8,T10:U11,T13:U14)</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="U17" s="18"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="19">
-        <f ca="1">AVERAGE(X7:Y8,X10:Y11,X13:Y14)</f>
-        <v>0</v>
-      </c>
-      <c r="Y17" s="19"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="20">
-        <f ca="1">AVERAGE(AA7:AB8,AA10:AB11,AA13:AB14)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="21">
-        <f ca="1">AVERAGE(AD7:AE8,AD10:AE11,AD13:AE14)</f>
-        <v>-0.75</v>
-      </c>
-      <c r="AE17" s="21"/>
-      <c r="AF17" s="1"/>
-      <c r="AG17" s="18">
-        <f ca="1">AVERAGE(AG7:AH8,AG10:AH11,AG13:AH14)</f>
-        <v>-0.83333333333333337</v>
-      </c>
-      <c r="AH17" s="18"/>
-      <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
-    </row>
-    <row r="18" spans="5:36">
-      <c r="E18" s="1"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="20"/>
-      <c r="AB18" s="20"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="21"/>
-      <c r="AE18" s="21"/>
-      <c r="AF18" s="1"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="1"/>
-      <c r="AJ18" s="1"/>
-    </row>
-    <row r="19" spans="5:36">
-      <c r="E19" s="1"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
-      <c r="AH19" s="1"/>
-      <c r="AI19" s="1"/>
-      <c r="AJ19" s="1"/>
-    </row>
-    <row r="20" spans="5:36">
-      <c r="E20" s="1"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="19">
-        <f ca="1">_xlfn.VAR.P(K7:L8,K10:L11,K13:L14)</f>
-        <v>5</v>
-      </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="20">
-        <f ca="1">_xlfn.VAR.P(N7:O8,N10:O11,N13:O14)</f>
-        <v>5.5</v>
-      </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="21">
-        <f ca="1">_xlfn.VAR.P(Q7:R8,Q10:R11,Q13:R14)</f>
-        <v>2.3541666666666665</v>
-      </c>
-      <c r="R20" s="21"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="18">
-        <f ca="1">_xlfn.VAR.P(T7:U8,T10:U11,T13:U14)</f>
-        <v>4.5555555555555554</v>
-      </c>
-      <c r="U20" s="18"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="19">
-        <f ca="1">_xlfn.VAR.P(X7:Y8,X10:Y11,X13:Y14)</f>
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="Y20" s="19"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="20">
-        <f ca="1">_xlfn.VAR.P(AA7:AB8,AA10:AB11,AA13:AB14)</f>
-        <v>3.5555555555555554</v>
-      </c>
-      <c r="AB20" s="20"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="21">
-        <f ca="1">_xlfn.VAR.P(AD7:AE8,AD10:AE11,AD13:AE14)</f>
-        <v>5.020833333333333</v>
-      </c>
-      <c r="AE20" s="21"/>
-      <c r="AF20" s="1"/>
-      <c r="AG20" s="18">
-        <f ca="1">_xlfn.VAR.P(AG7:AH8,AG10:AH11,AG13:AH14)</f>
-        <v>2.8055555555555554</v>
-      </c>
-      <c r="AH20" s="18"/>
-      <c r="AI20" s="1"/>
-      <c r="AJ20" s="1"/>
-    </row>
-    <row r="21" spans="5:36">
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="20"/>
-      <c r="AB21" s="20"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="21"/>
-      <c r="AE21" s="21"/>
-      <c r="AF21" s="1"/>
-      <c r="AG21" s="18"/>
-      <c r="AH21" s="18"/>
-      <c r="AI21" s="1"/>
-      <c r="AJ21" s="1"/>
-    </row>
-    <row r="22" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-      <c r="AE22" s="1"/>
-      <c r="AF22" s="1"/>
-      <c r="AG22" s="1"/>
-      <c r="AH22" s="1"/>
-      <c r="AI22" s="1"/>
-      <c r="AJ22" s="1"/>
-    </row>
-    <row r="23" spans="5:36">
-      <c r="E23" s="1"/>
-      <c r="F23" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="24">
-        <f ca="1">AVERAGE(K7:U8)</f>
-        <v>0.4375</v>
-      </c>
-      <c r="L23" s="25"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="24">
-        <f ca="1">AVERAGE(K10:U11)</f>
-        <v>0.4375</v>
-      </c>
-      <c r="O23" s="25"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="24">
-        <f ca="1">AVERAGE(K13:U14)</f>
-        <v>-0.1875</v>
-      </c>
-      <c r="R23" s="25"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="24">
-        <f ca="1">AVERAGE(X7:AH8)</f>
-        <v>-0.625</v>
-      </c>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="24">
-        <f ca="1">AVERAGE(X10:AH11)</f>
-        <v>0.5625</v>
-      </c>
-      <c r="AB23" s="25"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="24">
-        <f ca="1">AVERAGE(X13:AH14)</f>
-        <v>-0.875</v>
-      </c>
-      <c r="AE23" s="25"/>
-      <c r="AF23" s="1"/>
-      <c r="AG23" s="1"/>
-      <c r="AH23" s="1"/>
-      <c r="AI23" s="1"/>
-      <c r="AJ23" s="1"/>
-    </row>
-    <row r="24" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E24" s="1"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="27"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="26"/>
-      <c r="AE24" s="27"/>
-      <c r="AF24" s="1"/>
-      <c r="AG24" s="1"/>
-      <c r="AH24" s="1"/>
-      <c r="AI24" s="1"/>
-      <c r="AJ24" s="1"/>
-    </row>
-    <row r="25" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E25" s="1"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="1"/>
-      <c r="AF25" s="1"/>
-      <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
-      <c r="AI25" s="1"/>
-      <c r="AJ25" s="1"/>
-    </row>
-    <row r="26" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E26" s="1"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="24">
-        <f ca="1">_xlfn.VAR.P(K7:U8)</f>
-        <v>5.74609375</v>
-      </c>
-      <c r="L26" s="25"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="24">
-        <f ca="1">_xlfn.VAR.P(K10:U11)</f>
-        <v>5.87109375</v>
-      </c>
-      <c r="O26" s="25"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="24">
-        <f ca="1">_xlfn.VAR.P(K13:U14)</f>
-        <v>6.65234375</v>
-      </c>
-      <c r="R26" s="25"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="24">
-        <f ca="1">_xlfn.VAR.P(X7:AH8)</f>
-        <v>2.609375</v>
-      </c>
-      <c r="Y26" s="25"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="24">
-        <f ca="1">_xlfn.VAR.P(X10:AH11)</f>
-        <v>3.74609375</v>
-      </c>
-      <c r="AB26" s="25"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="24">
-        <f ca="1">_xlfn.VAR.P(X13:AH14)</f>
-        <v>3.484375</v>
-      </c>
-      <c r="AE26" s="25"/>
-      <c r="AF26" s="1"/>
-      <c r="AG26" s="1"/>
-      <c r="AH26" s="1"/>
-      <c r="AI26" s="1"/>
-      <c r="AJ26" s="1"/>
-    </row>
-    <row r="27" spans="5:36" ht="16.2" thickBot="1">
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="26"/>
-      <c r="Y27" s="27"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="27"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="26"/>
-      <c r="AE27" s="27"/>
-      <c r="AF27" s="1"/>
-      <c r="AG27" s="1"/>
-      <c r="AH27" s="1"/>
-      <c r="AI27" s="1"/>
-      <c r="AJ27" s="1"/>
-    </row>
-    <row r="28" spans="5:36">
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
-      <c r="AI28" s="1"/>
-      <c r="AJ28" s="1"/>
-    </row>
-    <row r="29" spans="5:36">
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
-      <c r="AE29" s="1"/>
-      <c r="AF29" s="1"/>
-      <c r="AG29" s="1"/>
-      <c r="AH29" s="1"/>
-      <c r="AI29" s="1"/>
-      <c r="AJ29" s="1"/>
-    </row>
-    <row r="30" spans="5:36">
-      <c r="E30" s="1"/>
-      <c r="F30" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="34"/>
-      <c r="H30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I30" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="23">
-        <f ca="1">AVERAGE(K7:O8)</f>
-        <v>0.875</v>
-      </c>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="23">
-        <f ca="1">AVERAGE(Q7:U8)</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="23">
-        <f ca="1">AVERAGE(X7:AB8)</f>
-        <v>-0.25</v>
-      </c>
-      <c r="Y30" s="23"/>
-      <c r="Z30" s="23"/>
-      <c r="AA30" s="23"/>
-      <c r="AB30" s="23"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="23">
-        <f ca="1">AVERAGE(AD7:AH8)</f>
-        <v>-1</v>
-      </c>
-      <c r="AE30" s="23"/>
-      <c r="AF30" s="23"/>
-      <c r="AG30" s="23"/>
-      <c r="AH30" s="23"/>
-      <c r="AI30" s="1"/>
-      <c r="AJ30" s="1"/>
-    </row>
-    <row r="31" spans="5:36">
-      <c r="E31" s="1"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="23">
-        <f ca="1">AVERAGE(K10:O11)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="23">
-        <f ca="1">AVERAGE(Q10:U11)</f>
-        <v>-0.625</v>
-      </c>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="23">
-        <f ca="1">AVERAGE(X10:AB11)</f>
-        <v>0.75</v>
-      </c>
-      <c r="Y31" s="23"/>
-      <c r="Z31" s="23"/>
-      <c r="AA31" s="23"/>
-      <c r="AB31" s="23"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="23">
-        <f ca="1">AVERAGE(AD10:AH11)</f>
-        <v>0.375</v>
-      </c>
-      <c r="AE31" s="23"/>
-      <c r="AF31" s="23"/>
-      <c r="AG31" s="23"/>
-      <c r="AH31" s="23"/>
-      <c r="AI31" s="1"/>
-      <c r="AJ31" s="1"/>
-    </row>
-    <row r="32" spans="5:36">
-      <c r="E32" s="1"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="23">
-        <f ca="1">AVERAGE(K13:O14)</f>
-        <v>0.625</v>
-      </c>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="23">
-        <f ca="1">AVERAGE(Q13:U14)</f>
-        <v>-1</v>
-      </c>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="23">
-        <f ca="1">AVERAGE(X13:AB14)</f>
-        <v>0</v>
-      </c>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="23">
-        <f ca="1">AVERAGE(AD13:AH14)</f>
-        <v>-1.75</v>
-      </c>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="23"/>
-      <c r="AG32" s="23"/>
-      <c r="AH32" s="23"/>
-      <c r="AI32" s="1"/>
-      <c r="AJ32" s="1"/>
-    </row>
-    <row r="33" spans="5:36">
-      <c r="E33" s="1"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+    <row r="33" spans="10:38">
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-      <c r="AE33" s="1"/>
-      <c r="AF33" s="1"/>
-      <c r="AG33" s="1"/>
-      <c r="AH33" s="1"/>
-      <c r="AI33" s="1"/>
-      <c r="AJ33" s="1"/>
     </row>
-    <row r="34" spans="5:36">
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
+    <row r="34" spans="10:38">
+      <c r="L34" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="M34" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="23">
-        <f ca="1">_xlfn.VAR.P(K7:O8)</f>
-        <v>6.109375</v>
-      </c>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="23">
-        <f ca="1">_xlfn.VAR.P(Q7:U8)</f>
-        <v>5</v>
-      </c>
-      <c r="R34" s="23"/>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="23"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="23">
-        <f ca="1">_xlfn.VAR.P(X7:AB8)</f>
-        <v>1.9375</v>
-      </c>
-      <c r="Y34" s="23"/>
-      <c r="Z34" s="23"/>
-      <c r="AA34" s="23"/>
-      <c r="AB34" s="23"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="23">
-        <f ca="1">_xlfn.VAR.P(AD7:AH8)</f>
-        <v>3</v>
-      </c>
-      <c r="AE34" s="23"/>
-      <c r="AF34" s="23"/>
-      <c r="AG34" s="23"/>
-      <c r="AH34" s="23"/>
-      <c r="AI34" s="1"/>
-      <c r="AJ34" s="1"/>
+      <c r="O34" s="10">
+        <f ca="1">_xlfn.VAR.P(O7:S8)</f>
+        <v>5.25</v>
+      </c>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="U34" s="10">
+        <f ca="1">_xlfn.VAR.P(U7:Y8)</f>
+        <v>4.25</v>
+      </c>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="AB34" s="10">
+        <f ca="1">_xlfn.VAR.P(AB7:AF8)</f>
+        <v>4.4375</v>
+      </c>
+      <c r="AC34" s="10"/>
+      <c r="AD34" s="10"/>
+      <c r="AE34" s="10"/>
+      <c r="AF34" s="10"/>
+      <c r="AH34" s="10">
+        <f ca="1">_xlfn.VAR.P(AH7:AL8)</f>
+        <v>4.109375</v>
+      </c>
+      <c r="AI34" s="10"/>
+      <c r="AJ34" s="10"/>
+      <c r="AK34" s="10"/>
+      <c r="AL34" s="10"/>
     </row>
-    <row r="35" spans="5:36">
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="23">
-        <f ca="1">_xlfn.VAR.P(K10:O11)</f>
-        <v>4.5</v>
-      </c>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="23">
-        <f ca="1">_xlfn.VAR.P(Q10:U11)</f>
-        <v>4.984375</v>
-      </c>
-      <c r="R35" s="23"/>
-      <c r="S35" s="23"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="23"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="23">
-        <f ca="1">_xlfn.VAR.P(X10:AB11)</f>
-        <v>2.4375</v>
-      </c>
-      <c r="Y35" s="23"/>
-      <c r="Z35" s="23"/>
-      <c r="AA35" s="23"/>
-      <c r="AB35" s="23"/>
-      <c r="AC35" s="1"/>
-      <c r="AD35" s="23">
-        <f ca="1">_xlfn.VAR.P(AD10:AH11)</f>
-        <v>4.984375</v>
-      </c>
-      <c r="AE35" s="23"/>
-      <c r="AF35" s="23"/>
-      <c r="AG35" s="23"/>
-      <c r="AH35" s="23"/>
-      <c r="AI35" s="1"/>
-      <c r="AJ35" s="1"/>
+    <row r="35" spans="10:38">
+      <c r="O35" s="10">
+        <f ca="1">_xlfn.VAR.P(O10:S11)</f>
+        <v>6.6875</v>
+      </c>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="U35" s="10">
+        <f ca="1">_xlfn.VAR.P(U10:Y11)</f>
+        <v>4.359375</v>
+      </c>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="AB35" s="10">
+        <f ca="1">_xlfn.VAR.P(AB10:AF11)</f>
+        <v>3.6875</v>
+      </c>
+      <c r="AC35" s="10"/>
+      <c r="AD35" s="10"/>
+      <c r="AE35" s="10"/>
+      <c r="AF35" s="10"/>
+      <c r="AH35" s="10">
+        <f ca="1">_xlfn.VAR.P(AH10:AL11)</f>
+        <v>3.359375</v>
+      </c>
+      <c r="AI35" s="10"/>
+      <c r="AJ35" s="10"/>
+      <c r="AK35" s="10"/>
+      <c r="AL35" s="10"/>
     </row>
-    <row r="36" spans="5:36">
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="23">
-        <f ca="1">_xlfn.VAR.P(K13:O14)</f>
-        <v>7.734375</v>
-      </c>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="23">
-        <f ca="1">_xlfn.VAR.P(Q13:U14)</f>
-        <v>4.25</v>
-      </c>
-      <c r="R36" s="23"/>
-      <c r="S36" s="23"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="23"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="23">
-        <f ca="1">_xlfn.VAR.P(X13:AB14)</f>
-        <v>4</v>
-      </c>
-      <c r="Y36" s="23"/>
-      <c r="Z36" s="23"/>
-      <c r="AA36" s="23"/>
-      <c r="AB36" s="23"/>
-      <c r="AC36" s="1"/>
-      <c r="AD36" s="23">
-        <f ca="1">_xlfn.VAR.P(AD13:AH14)</f>
-        <v>1.4375</v>
-      </c>
-      <c r="AE36" s="23"/>
-      <c r="AF36" s="23"/>
-      <c r="AG36" s="23"/>
-      <c r="AH36" s="23"/>
-      <c r="AI36" s="1"/>
-      <c r="AJ36" s="1"/>
-    </row>
-    <row r="37" spans="5:36">
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="1"/>
-      <c r="AD37" s="1"/>
-      <c r="AE37" s="1"/>
-      <c r="AF37" s="1"/>
-      <c r="AG37" s="1"/>
-      <c r="AH37" s="1"/>
-      <c r="AI37" s="1"/>
-      <c r="AJ37" s="1"/>
+    <row r="36" spans="10:38">
+      <c r="O36" s="10">
+        <f ca="1">_xlfn.VAR.P(O13:S14)</f>
+        <v>4.75</v>
+      </c>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="U36" s="10">
+        <f ca="1">_xlfn.VAR.P(U13:Y14)</f>
+        <v>2.859375</v>
+      </c>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="10"/>
+      <c r="AB36" s="10">
+        <f ca="1">_xlfn.VAR.P(AB13:AF14)</f>
+        <v>5.4375</v>
+      </c>
+      <c r="AC36" s="10"/>
+      <c r="AD36" s="10"/>
+      <c r="AE36" s="10"/>
+      <c r="AF36" s="10"/>
+      <c r="AH36" s="10">
+        <f ca="1">_xlfn.VAR.P(AH13:AL14)</f>
+        <v>3.984375</v>
+      </c>
+      <c r="AI36" s="10"/>
+      <c r="AJ36" s="10"/>
+      <c r="AK36" s="10"/>
+      <c r="AL36" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="K36:O36"/>
-    <mergeCell ref="Q36:U36"/>
-    <mergeCell ref="X36:AB36"/>
-    <mergeCell ref="AD36:AH36"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="K34:O34"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="X34:AB34"/>
-    <mergeCell ref="K35:O35"/>
-    <mergeCell ref="Q35:U35"/>
-    <mergeCell ref="X35:AB35"/>
-    <mergeCell ref="AD35:AH35"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="X32:AB32"/>
-    <mergeCell ref="AD32:AH32"/>
-    <mergeCell ref="AD34:AH34"/>
-    <mergeCell ref="X31:AB31"/>
-    <mergeCell ref="AD31:AH31"/>
-    <mergeCell ref="AD30:AH30"/>
-    <mergeCell ref="K30:O30"/>
-    <mergeCell ref="F30:G33"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="K31:O31"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="AA26:AB27"/>
-    <mergeCell ref="AD26:AE27"/>
-    <mergeCell ref="X23:Y24"/>
-    <mergeCell ref="AA23:AB24"/>
-    <mergeCell ref="AD23:AE24"/>
-    <mergeCell ref="K26:L27"/>
-    <mergeCell ref="N26:O27"/>
-    <mergeCell ref="Q26:R27"/>
-    <mergeCell ref="X26:Y27"/>
-    <mergeCell ref="F23:G26"/>
-    <mergeCell ref="K23:L24"/>
-    <mergeCell ref="N23:O24"/>
-    <mergeCell ref="Q23:R24"/>
-    <mergeCell ref="F7:G14"/>
-    <mergeCell ref="K17:L18"/>
-    <mergeCell ref="K20:L21"/>
-    <mergeCell ref="N17:O18"/>
-    <mergeCell ref="Q17:R18"/>
-    <mergeCell ref="N20:O21"/>
-    <mergeCell ref="Q20:R21"/>
-    <mergeCell ref="F17:G20"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K4:U4"/>
-    <mergeCell ref="X4:AH4"/>
-    <mergeCell ref="T17:U18"/>
-    <mergeCell ref="T20:U21"/>
+  <mergeCells count="83">
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="E12:F13"/>
+    <mergeCell ref="G12:H13"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="G14:H15"/>
+    <mergeCell ref="O4:Y4"/>
+    <mergeCell ref="AB4:AL4"/>
     <mergeCell ref="X17:Y18"/>
     <mergeCell ref="X20:Y21"/>
-    <mergeCell ref="AA17:AB18"/>
-    <mergeCell ref="AA20:AB21"/>
-    <mergeCell ref="AD17:AE18"/>
-    <mergeCell ref="AD20:AE21"/>
-    <mergeCell ref="AG17:AH18"/>
-    <mergeCell ref="AG20:AH21"/>
+    <mergeCell ref="AB17:AC18"/>
+    <mergeCell ref="AB20:AC21"/>
+    <mergeCell ref="AE17:AF18"/>
+    <mergeCell ref="AE20:AF21"/>
+    <mergeCell ref="AH17:AI18"/>
+    <mergeCell ref="AH20:AI21"/>
+    <mergeCell ref="AK17:AL18"/>
+    <mergeCell ref="AK20:AL21"/>
+    <mergeCell ref="J7:K14"/>
+    <mergeCell ref="O17:P18"/>
+    <mergeCell ref="O20:P21"/>
+    <mergeCell ref="R17:S18"/>
+    <mergeCell ref="U17:V18"/>
+    <mergeCell ref="R20:S21"/>
+    <mergeCell ref="U20:V21"/>
+    <mergeCell ref="J17:K20"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="O26:P27"/>
+    <mergeCell ref="R26:S27"/>
+    <mergeCell ref="U26:V27"/>
+    <mergeCell ref="AB26:AC27"/>
+    <mergeCell ref="J23:K26"/>
+    <mergeCell ref="O23:P24"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="U23:V24"/>
+    <mergeCell ref="AE26:AF27"/>
+    <mergeCell ref="AH26:AI27"/>
+    <mergeCell ref="AB23:AC24"/>
+    <mergeCell ref="AE23:AF24"/>
+    <mergeCell ref="AH23:AI24"/>
+    <mergeCell ref="J30:K33"/>
+    <mergeCell ref="U30:Y30"/>
+    <mergeCell ref="AB30:AF30"/>
+    <mergeCell ref="O31:S31"/>
+    <mergeCell ref="U31:Y31"/>
+    <mergeCell ref="AH34:AL34"/>
+    <mergeCell ref="AB31:AF31"/>
+    <mergeCell ref="AH31:AL31"/>
+    <mergeCell ref="AH30:AL30"/>
+    <mergeCell ref="O30:S30"/>
+    <mergeCell ref="O36:S36"/>
+    <mergeCell ref="U36:Y36"/>
+    <mergeCell ref="AB36:AF36"/>
+    <mergeCell ref="AH36:AL36"/>
+    <mergeCell ref="M30:M32"/>
+    <mergeCell ref="O34:S34"/>
+    <mergeCell ref="U34:Y34"/>
+    <mergeCell ref="AB34:AF34"/>
+    <mergeCell ref="O35:S35"/>
+    <mergeCell ref="U35:Y35"/>
+    <mergeCell ref="AB35:AF35"/>
+    <mergeCell ref="AH35:AL35"/>
+    <mergeCell ref="O32:S32"/>
+    <mergeCell ref="U32:Y32"/>
+    <mergeCell ref="AB32:AF32"/>
+    <mergeCell ref="AH32:AL32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>